<commit_message>
add data calculator service and logic & interfaces
</commit_message>
<xml_diff>
--- a/src/assets/DW_Mini_case.xlsx
+++ b/src/assets/DW_Mini_case.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\projects\angular\awesome-pharma\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D38F492D-10C3-4DB0-86C2-F2A744A83F2C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B401E324-D3DC-4D08-986C-EA5B92AEDD79}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="2" xr2:uid="{98052005-1074-4499-820C-2E6BD8DF5FAB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="3" xr2:uid="{98052005-1074-4499-820C-2E6BD8DF5FAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Salesperson" sheetId="1" r:id="rId1"/>
@@ -1250,7 +1250,7 @@
   <dimension ref="A1:G809"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E700" sqref="E1:E1048576"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19262,8 +19262,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AAFBD41-A4CD-4705-9069-A2974D5A59F2}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19450,7 +19450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154909EE-F61E-4759-BB18-92485F3E3629}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>